<commit_message>
met a jour les stories
</commit_message>
<xml_diff>
--- a/excel/Stories-SpicyNvaders-theorlando.xlsx
+++ b/excel/Stories-SpicyNvaders-theorlando.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theorlando\Documents\GitHub\Spicy-Nvader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theorlando\Documents\GitHub\Spicy-Nvader\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9634BC-847E-4307-B59F-71B11082E5B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4D0F28-28C3-442C-A41E-5A2F71A6EBBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{FC1220D0-F500-4509-AEBD-73DE32FF46A9}"/>
+    <workbookView xWindow="3060" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{FC1220D0-F500-4509-AEBD-73DE32FF46A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -111,11 +111,6 @@
 Afin que mon highscore s'affiche dans le menu "HIGHSCORES"</t>
   </si>
   <si>
-    <t>En tant que joueur sur la page d'entrée de pseudo
-En pressant entrée le pseudo s'enregistre
-Pour savoir qui vas jouer</t>
-  </si>
-  <si>
     <t>Lancement de la partie</t>
   </si>
   <si>
@@ -124,32 +119,6 @@
 Pour pouvoir jouer dans de bonnes condition</t>
   </si>
   <si>
-    <t xml:space="preserve">En tant que joueur au lancement de la partie
-le compteur de vie s'affiche avec toute les vies
-Pour savoir combien de vie il me reste
-</t>
-  </si>
-  <si>
-    <t>En tant que joueur au lancement de la partie
-Les murs s'affichent entierement construit
-Pour pouvoir me protéger des aliens</t>
-  </si>
-  <si>
-    <t>En tant que joueur au lancement de la partie
-Le vaisseau du joueur s'affiche 
-Pour pouvoir tirer sur les aliens</t>
-  </si>
-  <si>
-    <t>En tant que joueur au lancement de la partie
-Le compteur de score s'affiche
-pour savoir mon score en temps réel</t>
-  </si>
-  <si>
-    <t>En tant que joueur au lancement de la partie
-les aliens s'affichent
-Pour pouvoir tirer sur les aliens et qu'ils nous tirent dessus</t>
-  </si>
-  <si>
     <t>Tir des aliens</t>
   </si>
   <si>
@@ -176,12 +145,6 @@
     <t>dans le menu option avec le curseur sur l'option de difficulté sélectionnée,
 a la pression de la flèche gauche
 la difficulté change (facile -&gt;  godmod -&gt; difficile -&gt; moyen -&gt; facile)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quand l'entrée "PLAY" sur le menu principale est choisi
-une page d'entrée de pseudo s'affichage
-Pour pouvoir rentrer mon pseudo
-</t>
   </si>
   <si>
     <t>dans le menu option avec le curseur sur l'option de son sélectionnée,
@@ -413,6 +376,42 @@
     <t>Dans le menu principale
 Quand je choisi le menu about
 Le menu about s'affiche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quand l'entrée "PLAY" sur le menu principale est choisi
+a la pression de entrer
+une page d'entrée de pseudo s'affichage
+</t>
+  </si>
+  <si>
+    <t>sur la page d'entrée de pseudo
+En pressant entrer
+le jeu se lance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">au lancement de la partie
+Les murs s'affichent entierement construit (5)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">au lancement de la partie
+le compteur de vie s'affiche en haut a gauche avec toute les vies (3)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">au lancement de la partie
+Le vaisseau du joueur s'affiche au centre en dessous des murs
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">au lancement de la partie
+Le compteur de score s'affiche en haut a droite
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">au lancement de la partie
+les aliens s'affichent (3 ligne et 7 par ligne)
+</t>
   </si>
 </sst>
 </file>
@@ -602,8 +601,8 @@
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>243876</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>443901</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -944,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980F9A3D-880B-4EDA-9E11-7E060A805D83}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,7 +988,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -1031,10 +1030,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -1054,10 +1053,10 @@
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1065,18 +1064,18 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1084,40 +1083,40 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1128,22 +1127,22 @@
     </row>
     <row r="10" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1151,16 +1150,16 @@
     </row>
     <row r="11" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1170,16 +1169,16 @@
     </row>
     <row r="12" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1189,16 +1188,16 @@
     </row>
     <row r="13" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1208,16 +1207,16 @@
     </row>
     <row r="14" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1227,13 +1226,13 @@
     </row>
     <row r="15" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1244,16 +1243,16 @@
     </row>
     <row r="16" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1263,22 +1262,22 @@
     </row>
     <row r="17" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1286,16 +1285,16 @@
     </row>
     <row r="18" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1305,16 +1304,16 @@
     </row>
     <row r="19" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1324,16 +1323,16 @@
     </row>
     <row r="20" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1484,6 +1483,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B4B9E7C5D694AD43BF578BC0F90B54B2" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="0984db86dc07217f5a46f514afe4bde0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2355ee30-94b2-4a5a-b7d7-59ce3ea1eb14" xmlns:ns4="46b00e57-26a5-4c78-86b9-22a327b96dfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="460f8b61d47669917f380c5230989cdf" ns3:_="" ns4:_="">
     <xsd:import namespace="2355ee30-94b2-4a5a-b7d7-59ce3ea1eb14"/>
@@ -1694,15 +1702,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1710,6 +1709,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0912D6D1-7DC0-4CFF-8ECC-C25F094057A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{590D46E6-F198-420C-846C-2B80001D3859}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1724,14 +1731,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0912D6D1-7DC0-4CFF-8ECC-C25F094057A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
met a jours les stories
</commit_message>
<xml_diff>
--- a/excel/Stories-SpicyNvaders-theorlando.xlsx
+++ b/excel/Stories-SpicyNvaders-theorlando.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theorlando\Documents\GitHub\Spicy-Nvader\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4D0F28-28C3-442C-A41E-5A2F71A6EBBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D81C1C6-F065-4565-8ED7-6D9446684250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{FC1220D0-F500-4509-AEBD-73DE32FF46A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC1220D0-F500-4509-AEBD-73DE32FF46A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="83">
   <si>
     <t>titre</t>
   </si>
@@ -190,11 +190,6 @@
 pour savoir combien de fois j'ai encore droit a l'erreur</t>
   </si>
   <si>
-    <t>Quand un tir alien touche le vaisseau du joueur
-le compteur fait disparaitre une vie
-Pour que le joueur perde une vie</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 </t>
   </si>
@@ -244,11 +239,6 @@
 Afin de battre mon highscore</t>
   </si>
   <si>
-    <t>Quand un alien est détruit 
-il rapporte des points
-pour pouvoir augmenté mon score</t>
-  </si>
-  <si>
     <t>Aliens détruit</t>
   </si>
   <si>
@@ -265,12 +255,6 @@
     <t>Tout les aliens détruit</t>
   </si>
   <si>
-    <t xml:space="preserve">Quand le vaisseau du joueur est touché
-Le joueur pert des points
-Pour pénalisé les joueur qui se font beaucoup touché
-</t>
-  </si>
-  <si>
     <t>En tant que joueur
 Je veux que le jeu réagisse a la mort d'une vague entière d'aliens
 Pour pouvoir continuer à jouer et être récompensé</t>
@@ -294,26 +278,9 @@
     <t>Déplacement du vaisseau du joueur</t>
   </si>
   <si>
-    <t xml:space="preserve">Quand la flèche de droite est préssée en jeu
-Le vaisseau se déplace sur la droite
-Pour pouvoir me déplacer
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quand la flèche de gauche est préssée en jeu
-Le vaisseau se déplace sur la gauche
-Pour pouvoir me déplacer
-</t>
-  </si>
-  <si>
     <t>En tant que joueur 
 Je veux pouvoir déplacer mon vaisseau de manière horizontal
 Pour pouvoir esquiver les tirs ennemis et me positionné pour tirer  sur les ennemis</t>
-  </si>
-  <si>
-    <t>Quand une flèche directionel est appuyée longuement
-Le vaisseau se déplace de manière continue dans la direction séléctionée
-Pour facilité les déplacement de joueur</t>
   </si>
   <si>
     <t>Tir du vaisseau du joueur</t>
@@ -411,6 +378,43 @@
   <si>
     <t xml:space="preserve">au lancement de la partie
 les aliens s'affichent (3 ligne et 7 par ligne)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Un tir alien touche le vaisseau du joueur
+le compteur fait disparaitre une vie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">un alien est détruit 
+il augmente le compteur de sa valeur en points
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le vaisseau du joueur est touché
+Le joueur pert des points
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En jeu
+la flèche de droite est préssée 
+Le vaisseau se déplace sur la droite
+</t>
+  </si>
+  <si>
+    <t>En jeu
+la flèche de gauche est préssée 
+Le vaisseau se déplace sur la gauche</t>
+  </si>
+  <si>
+    <t>En jeu
+Quand une flèche directionel est appuyée longuement
+Le vaisseau se déplace de manière continue dans la direction séléctionée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En jeu
+le vaisseau arrive au bord de l'écran
+Le vaisseau ne peut plus se déplacer vers le côté ou il est déjà collé au bord
 </t>
   </si>
 </sst>
@@ -441,7 +445,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,6 +461,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -571,6 +581,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -943,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980F9A3D-880B-4EDA-9E11-7E060A805D83}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,10 +1085,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1091,19 +1104,19 @@
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -1142,24 +1155,24 @@
         <v>32</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1169,16 +1182,16 @@
     </row>
     <row r="12" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1188,16 +1201,16 @@
     </row>
     <row r="13" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1205,18 +1218,18 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1226,13 +1239,13 @@
     </row>
     <row r="15" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1243,16 +1256,16 @@
     </row>
     <row r="16" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1262,22 +1275,22 @@
     </row>
     <row r="17" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1285,16 +1298,16 @@
     </row>
     <row r="18" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1304,16 +1317,16 @@
     </row>
     <row r="19" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1323,16 +1336,16 @@
     </row>
     <row r="20" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1483,15 +1496,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B4B9E7C5D694AD43BF578BC0F90B54B2" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="0984db86dc07217f5a46f514afe4bde0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2355ee30-94b2-4a5a-b7d7-59ce3ea1eb14" xmlns:ns4="46b00e57-26a5-4c78-86b9-22a327b96dfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="460f8b61d47669917f380c5230989cdf" ns3:_="" ns4:_="">
     <xsd:import namespace="2355ee30-94b2-4a5a-b7d7-59ce3ea1eb14"/>
@@ -1702,6 +1706,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1709,14 +1722,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0912D6D1-7DC0-4CFF-8ECC-C25F094057A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{590D46E6-F198-420C-846C-2B80001D3859}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1731,6 +1736,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0912D6D1-7DC0-4CFF-8ECC-C25F094057A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
met a jour le déplacement des alien
</commit_message>
<xml_diff>
--- a/excel/Stories-SpicyNvaders-theorlando.xlsx
+++ b/excel/Stories-SpicyNvaders-theorlando.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theorlando\Documents\GitHub\Spicy-Nvader\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D81C1C6-F065-4565-8ED7-6D9446684250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF90123-6431-4645-AF32-5D7C6D81BC48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC1220D0-F500-4509-AEBD-73DE32FF46A9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
   <si>
     <t>titre</t>
   </si>
@@ -322,11 +322,6 @@
 </t>
   </si>
   <si>
-    <t>Quand le vaisseau arrive au bord de l'écran
-Le vaisseau ne peut plus se déplacer vers le côté ou il est déjà collé au bord
-Afin que le vaisseau ne disparaisse pas de l'écran</t>
-  </si>
-  <si>
     <t>Menu About</t>
   </si>
   <si>
@@ -381,21 +376,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
-Un tir alien touche le vaisseau du joueur
-le compteur fait disparaitre une vie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">un alien est détruit 
-il augmente le compteur de sa valeur en points
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">le vaisseau du joueur est touché
-Le joueur pert des points
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">En jeu
 la flèche de droite est préssée 
 Le vaisseau se déplace sur la droite
@@ -415,6 +395,30 @@
     <t xml:space="preserve">En jeu
 le vaisseau arrive au bord de l'écran
 Le vaisseau ne peut plus se déplacer vers le côté ou il est déjà collé au bord
+</t>
+  </si>
+  <si>
+    <t>Un tir alien touche le vaisseau du joueur
+le compteur fait disparaitre une vie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">un alien de type A est détruit 
+le score augmente de 10 points
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">un alien de type B est détruit 
+le score augmente de 20 points
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">un alien de type C est détruit 
+le score augmente de 30 points
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le vaisseau du joueur est touché
+Le joueur pert des points (100)
 </t>
   </si>
 </sst>
@@ -445,7 +449,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,12 +465,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -581,9 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -956,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980F9A3D-880B-4EDA-9E11-7E060A805D83}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,10 +1080,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1104,19 +1099,19 @@
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -1162,14 +1157,14 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>35</v>
@@ -1219,20 +1214,24 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1274,23 +1273,23 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1336,16 +1335,16 @@
     </row>
     <row r="20" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>

</xml_diff>

<commit_message>
mise en place du systeme de frames
</commit_message>
<xml_diff>
--- a/excel/Stories-SpicyNvaders-theorlando.xlsx
+++ b/excel/Stories-SpicyNvaders-theorlando.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theorlando\Documents\GitHub\Spicy-Nvader\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF90123-6431-4645-AF32-5D7C6D81BC48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7446C2-9DBF-4552-8CF7-CD6D39B18489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC1220D0-F500-4509-AEBD-73DE32FF46A9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
   <si>
     <t>titre</t>
   </si>
@@ -165,23 +165,6 @@
 Pour ajouter un atout a mon adversaire</t>
   </si>
   <si>
-    <t xml:space="preserve">Quand la partie est en cours
-Les aliens se déplacent vers la droite a un rythme régulier
-Pour faires bouger les aliens
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quand la partie est en cours
-Les aliens se déplacent vers la gauche a un rythme régulier
-Pour faires bouger les aliens
-</t>
-  </si>
-  <si>
-    <t>Quand les aliens arrivent au bord de l'écran
-Les aliens descende d'une ligne et reparte dans l'autre sens
-Pour que les aliens se rapproche petit à petit du joueur</t>
-  </si>
-  <si>
     <t>Compteur de vie</t>
   </si>
   <si>
@@ -270,11 +253,6 @@
 Pour récompensé le joueur d'avoir éliminé un vague entière d'énnemis</t>
   </si>
   <si>
-    <t>Quand les aliens se déplacent horizontalement 
-A chaque case parcourue le model visuel de l'alien change
-Afin de créer une petite animation de déplacement</t>
-  </si>
-  <si>
     <t>Déplacement du vaisseau du joueur</t>
   </si>
   <si>
@@ -291,18 +269,6 @@
 Pour pouvoir détruire les aliens</t>
   </si>
   <si>
-    <t xml:space="preserve">Quand la flèche haut est préssée en jeu
-Le vaisseau tir un laser vers le haut
-Pour pouvoir tirer sur les aliens
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quand un laser est tirer par le vaisseau du joueur
-Le vaisseau ne peut pas tirer d'autre laser pendant 1s
-Pour limiter le nombre de tir du joueur
-</t>
-  </si>
-  <si>
     <t>Tir sur les murs</t>
   </si>
   <si>
@@ -420,6 +386,40 @@
     <t xml:space="preserve">le vaisseau du joueur est touché
 Le joueur pert des points (100)
 </t>
+  </si>
+  <si>
+    <t>Quand la partie est en cours
+Les aliens se déplacent vers la droite a un rythme régulier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quand la partie est en cours
+Les aliens se déplacent vers la gauche a un rythme régulier
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En jeu
+Quand la flèche haut est préssée en jeu
+Le vaisseau tir un laser vers le haut
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quand un alien touche le bord de l'écran
+Les aliens descende d'une ligne et reparte dans l'autre sens
+</t>
+  </si>
+  <si>
+    <t>Le missile est tiré
+Il avance d'une case toute les quart de seconde vers le haut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le laser a été tirer il y a moins d'une seconde
+Quand la flèche haut est préssée en jeu
+il ne se passe rien
+</t>
+  </si>
+  <si>
+    <t>Le missile atteint le haut de l'écran
+il disparait</t>
   </si>
 </sst>
 </file>
@@ -951,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980F9A3D-880B-4EDA-9E11-7E060A805D83}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,10 +1080,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1099,19 +1099,19 @@
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -1134,40 +1134,38 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>53</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="F10" s="3"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1177,16 +1175,16 @@
     </row>
     <row r="12" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1196,16 +1194,16 @@
     </row>
     <row r="13" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1215,22 +1213,22 @@
     </row>
     <row r="14" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1238,13 +1236,13 @@
     </row>
     <row r="15" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1255,16 +1253,16 @@
     </row>
     <row r="16" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1274,58 +1272,62 @@
     </row>
     <row r="17" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>56</v>
+    <row r="18" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1335,16 +1337,16 @@
     </row>
     <row r="20" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1495,6 +1497,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B4B9E7C5D694AD43BF578BC0F90B54B2" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="0984db86dc07217f5a46f514afe4bde0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2355ee30-94b2-4a5a-b7d7-59ce3ea1eb14" xmlns:ns4="46b00e57-26a5-4c78-86b9-22a327b96dfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="460f8b61d47669917f380c5230989cdf" ns3:_="" ns4:_="">
     <xsd:import namespace="2355ee30-94b2-4a5a-b7d7-59ce3ea1eb14"/>
@@ -1705,15 +1716,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1721,6 +1723,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0912D6D1-7DC0-4CFF-8ECC-C25F094057A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{590D46E6-F198-420C-846C-2B80001D3859}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1735,14 +1745,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0912D6D1-7DC0-4CFF-8ECC-C25F094057A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
met en place le tir du vaisseau
</commit_message>
<xml_diff>
--- a/excel/Stories-SpicyNvaders-theorlando.xlsx
+++ b/excel/Stories-SpicyNvaders-theorlando.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theorlando\Documents\GitHub\Spicy-Nvader\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7446C2-9DBF-4552-8CF7-CD6D39B18489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B594DA-5238-4E11-AA7E-79CD92890FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC1220D0-F500-4509-AEBD-73DE32FF46A9}"/>
   </bookViews>
@@ -272,22 +272,6 @@
     <t>Tir sur les murs</t>
   </si>
   <si>
-    <t>En tant que joueur 
-Je veux que les murs soit déstruictible
-Pour offrir plus de possibilité de gameplay</t>
-  </si>
-  <si>
-    <t>Quand un tir touche un mur
-la partie du mur change de couleur ( blanc -&gt; rouge )
-Pour indiquer au joueur que le mur vas bientôt casser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quand un tir touche un mur endommagé
-La partie du mur disparait
-Afin de laisser passer les tirs
-</t>
-  </si>
-  <si>
     <t>Menu About</t>
   </si>
   <si>
@@ -420,6 +404,20 @@
   <si>
     <t>Le missile atteint le haut de l'écran
 il disparait</t>
+  </si>
+  <si>
+    <t>En tant que joueur 
+Je veux que les murs soit destructible 
+Pour offrir plus de possibilité de gameplay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quand un tir touche un mur
+Le mur change de couleur ( blanc -&gt;jaune -&gt; orange -&gt;rouge )
+</t>
+  </si>
+  <si>
+    <t>Quand un tir touche un mur rouge
+le mur disparait</t>
   </si>
 </sst>
 </file>
@@ -449,7 +447,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,6 +463,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -579,6 +583,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980F9A3D-880B-4EDA-9E11-7E060A805D83}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,10 +1087,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1099,19 +1106,19 @@
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -1141,13 +1148,13 @@
         <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="5"/>
@@ -1162,7 +1169,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>32</v>
@@ -1219,16 +1226,16 @@
         <v>42</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="E14" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1278,16 +1285,16 @@
         <v>51</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1301,33 +1308,33 @@
         <v>53</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="E18" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1337,16 +1344,16 @@
     </row>
     <row r="20" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1497,15 +1504,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B4B9E7C5D694AD43BF578BC0F90B54B2" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="0984db86dc07217f5a46f514afe4bde0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2355ee30-94b2-4a5a-b7d7-59ce3ea1eb14" xmlns:ns4="46b00e57-26a5-4c78-86b9-22a327b96dfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="460f8b61d47669917f380c5230989cdf" ns3:_="" ns4:_="">
     <xsd:import namespace="2355ee30-94b2-4a5a-b7d7-59ce3ea1eb14"/>
@@ -1716,6 +1714,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1723,14 +1730,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0912D6D1-7DC0-4CFF-8ECC-C25F094057A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{590D46E6-F198-420C-846C-2B80001D3859}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1745,6 +1744,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0912D6D1-7DC0-4CFF-8ECC-C25F094057A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>